<commit_message>
Save HSI, option for core temp/HSI depending on HSI range, some optimization for memory
</commit_message>
<xml_diff>
--- a/FellrnrFullScreenConfig.xlsx
+++ b/FellrnrFullScreenConfig.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ab69548fc84aee54/Coding/GitHub/FellrnrFullScreen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="8_{16969DAA-F5AA-4E5B-B4E5-E6E7651336D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F956F26B-D198-45E3-B75C-99F8936F7D9E}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="8_{16969DAA-F5AA-4E5B-B4E5-E6E7651336D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{11388D7C-3DA4-45DE-A776-B291AA198745}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{DA8DB765-6D8F-4300-9F19-048FAF9F2AE7}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{DA8DB765-6D8F-4300-9F19-048FAF9F2AE7}"/>
   </bookViews>
   <sheets>
     <sheet name="Configure Fellrnr DataField" sheetId="2" r:id="rId1"/>
@@ -1121,8 +1121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB5114B0-8F86-4666-AEB5-BA80DBA07690}">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1138,19 +1138,19 @@
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="str">
         <f>K7</f>
-        <v>ca,hrP,hr,pwr,pac,ca,uD,gAP,dF,sL,oP,g,alt,aP,ts</v>
+        <v>ca,hrP,hr,pwr,pac,dis,uD,gAP,dF,sL,oP,g,alt,ht,ts</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="str">
         <f>K16</f>
-        <v>ca,hrP,hr,pwr,pac,ca,uD,gAP,dF,sL,oP,g,alt,aP,ts</v>
+        <v>ca,hrP,hr,pwr,pac,dis,uD,gAP,dF,sL,oP,g,alt,aP,ts</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="str">
         <f>K24</f>
-        <v>ca,hrP,hr,pwr,pac,ca,uD,gAP,dF,sL,oP,g,alt,aP,ts</v>
+        <v>ca,hrP,hr,pwr,pac,dEl,uD,gAP,dF,sL,oP,g,alt,aP,ts</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
@@ -1191,7 +1191,7 @@
       <c r="J7" s="3"/>
       <c r="K7" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,G6:I12)</f>
-        <v>ca,hrP,hr,pwr,pac,ca,uD,gAP,dF,sL,oP,g,alt,aP,ts</v>
+        <v>ca,hrP,hr,pwr,pac,dis,uD,gAP,dF,sL,oP,g,alt,ht,ts</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
@@ -1202,7 +1202,7 @@
         <v>20</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="G8" s="3" t="str">
         <f>LOOKUP(B8,Lookup!$B:$B,Lookup!$A:$A)</f>
@@ -1214,7 +1214,7 @@
       </c>
       <c r="I8" s="3" t="str">
         <f>LOOKUP(D8,Lookup!$B:$B,Lookup!$A:$A)</f>
-        <v>ca</v>
+        <v>dis</v>
       </c>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
@@ -1275,7 +1275,7 @@
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="G11" s="3" t="str">
         <f>LOOKUP(B11,Lookup!$B:$B,Lookup!$A:$A)</f>
@@ -1284,7 +1284,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3" t="str">
         <f>LOOKUP(D11,Lookup!$B:$B,Lookup!$A:$A)</f>
-        <v>aP</v>
+        <v>ht</v>
       </c>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -1362,7 +1362,7 @@
       <c r="J16" s="3"/>
       <c r="K16" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,G15:I21)</f>
-        <v>ca,hrP,hr,pwr,pac,ca,uD,gAP,dF,sL,oP,g,alt,aP,ts</v>
+        <v>ca,hrP,hr,pwr,pac,dis,uD,gAP,dF,sL,oP,g,alt,aP,ts</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
@@ -1373,7 +1373,7 @@
         <v>20</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="G17" s="3" t="str">
         <f>LOOKUP(B17,Lookup!$B:$B,Lookup!$A:$A)</f>
@@ -1385,7 +1385,7 @@
       </c>
       <c r="I17" s="3" t="str">
         <f>LOOKUP(D17,Lookup!$B:$B,Lookup!$A:$A)</f>
-        <v>ca</v>
+        <v>dis</v>
       </c>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
@@ -1523,7 +1523,7 @@
       <c r="J24" s="3"/>
       <c r="K24" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,G23:I29)</f>
-        <v>ca,hrP,hr,pwr,pac,ca,uD,gAP,dF,sL,oP,g,alt,aP,ts</v>
+        <v>ca,hrP,hr,pwr,pac,dEl,uD,gAP,dF,sL,oP,g,alt,aP,ts</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
@@ -1534,7 +1534,7 @@
         <v>20</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G25" s="3" t="str">
         <f>LOOKUP(B25,Lookup!$B:$B,Lookup!$A:$A)</f>
@@ -1546,7 +1546,7 @@
       </c>
       <c r="I25" s="3" t="str">
         <f>LOOKUP(D25,Lookup!$B:$B,Lookup!$A:$A)</f>
-        <v>ca</v>
+        <v>dEl</v>
       </c>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
@@ -1658,7 +1658,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66DC8704-023E-4C44-8644-D5D7787AF753}">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>